<commit_message>
Atualização automática de SAO_LEOPOLDO.xlsx
</commit_message>
<xml_diff>
--- a/SAO_LEOPOLDO.xlsx
+++ b/SAO_LEOPOLDO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{88E97395-966E-4441-980C-3C03555A7D2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{565D1C25-A4AD-4984-9133-1099ADF0C512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1367,7 +1367,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{994B7B98-9F05-451E-9CA0-15EF9E7A6AA6}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{F277DB80-E679-4CE9-A281-B568D6E38B7B}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1397,10 +1397,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64BD2E58-F311-495B-855A-D50E6FBA1E2E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC9DD7C5-3C0A-47A1-B230-5F3EC9A5CA91}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1438,7 +1438,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28DB8828-B293-48BE-B4FA-791CCC88E0CE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA01998D-4108-417C-95DA-21A0000B5DFA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1501,7 +1501,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B24DF135-1D55-40C0-9835-5541F46B1DC8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0E36040-1851-49E8-B22B-8117577CB442}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1520,7 +1520,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BD3332B-7C10-962D-CD03-36A78506B0EE}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD1D51C0-AD72-D664-0775-7001692EC427}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1569,7 +1569,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2762143C-CC9C-A60A-5C39-D6C3A9A1CB2C}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6508E1C0-B00F-648F-E71B-0FA86D09A258}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1588,7 +1588,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BFCB8C1-2F28-AFB5-06BD-EB40A7DF2FEE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FF33ED0-56A5-AA0C-0786-A242C25F23DC}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1619,7 +1619,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{535BD256-3D78-5188-5908-0BDB127FCA54}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49C4DA87-A3F2-2616-617D-BE7A8F9E5186}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1650,7 +1650,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{746B2C9B-C4A4-0EC1-436C-A5D3E8BBE893}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7218C895-13AE-611C-2859-6277CCAD87F8}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1693,7 +1693,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C93BF7B-8DB6-4FBC-A2A6-09181DFFEB31}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{069FFFE5-9633-41BE-B361-D99D63A2CF88}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1731,7 +1731,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A743EAB-1663-4BA6-BD25-279E66FB1F80}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BE7E59A-BDC6-4F59-ABE2-8F903529E3E8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1774,7 +1774,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1521101-4A3B-4DA1-8384-9D1460080841}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{618182BE-04D0-4335-B268-F646E8DBBF94}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2087,7 +2087,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31F4F736-22B8-4CBA-A441-AA5DA5EEB71E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFC96899-4D28-479F-BA0E-0FE42D847E8D}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>